<commit_message>
Updates for SLC7a5 rebuttal
Updates to molecule lists and beatson scheme.
</commit_message>
<xml_diff>
--- a/molecules-lists/64_U13C-glutamine infusion all.xlsx
+++ b/molecules-lists/64_U13C-glutamine infusion all.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\DATA\NiCEMSI\People\Chelsea\Metabolite Lists\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\2020_Scripts for Data Processing\Git Repository (March 2020)\molecules-lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B230E73-1997-485B-9ECC-DC26A0382A76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{DA222FD2-02EA-429D-8431-AFA8895842CE}"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="28800" windowHeight="12225"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$257</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -230,8 +229,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,6 +364,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="33">
@@ -709,54 +722,56 @@
     <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Accent1 2" xfId="20" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="20% - Accent2 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
-    <cellStyle name="20% - Accent3 2" xfId="28" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="20% - Accent4 2" xfId="32" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
-    <cellStyle name="20% - Accent5 2" xfId="36" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
-    <cellStyle name="20% - Accent6 2" xfId="40" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
-    <cellStyle name="40% - Accent1 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
-    <cellStyle name="40% - Accent2 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
-    <cellStyle name="40% - Accent3 2" xfId="29" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="40% - Accent4 2" xfId="33" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
-    <cellStyle name="40% - Accent5 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
-    <cellStyle name="40% - Accent6 2" xfId="41" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
-    <cellStyle name="60% - Accent1 2" xfId="22" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
-    <cellStyle name="60% - Accent2 2" xfId="26" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
-    <cellStyle name="60% - Accent3 2" xfId="30" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
-    <cellStyle name="60% - Accent4 2" xfId="34" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
-    <cellStyle name="60% - Accent5 2" xfId="38" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
-    <cellStyle name="60% - Accent6 2" xfId="42" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
-    <cellStyle name="Accent1 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
-    <cellStyle name="Accent2 2" xfId="23" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
-    <cellStyle name="Accent3 2" xfId="27" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
-    <cellStyle name="Accent4 2" xfId="31" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
-    <cellStyle name="Accent5 2" xfId="35" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
-    <cellStyle name="Accent6 2" xfId="39" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
-    <cellStyle name="Bad 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
-    <cellStyle name="Calculation 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
-    <cellStyle name="Check Cell 2" xfId="14" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
-    <cellStyle name="Explanatory Text 2" xfId="17" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
-    <cellStyle name="Good 2" xfId="7" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
+    <cellStyle name="20% - Accent1 2" xfId="20"/>
+    <cellStyle name="20% - Accent2 2" xfId="24"/>
+    <cellStyle name="20% - Accent3 2" xfId="28"/>
+    <cellStyle name="20% - Accent4 2" xfId="32"/>
+    <cellStyle name="20% - Accent5 2" xfId="36"/>
+    <cellStyle name="20% - Accent6 2" xfId="40"/>
+    <cellStyle name="40% - Accent1 2" xfId="21"/>
+    <cellStyle name="40% - Accent2 2" xfId="25"/>
+    <cellStyle name="40% - Accent3 2" xfId="29"/>
+    <cellStyle name="40% - Accent4 2" xfId="33"/>
+    <cellStyle name="40% - Accent5 2" xfId="37"/>
+    <cellStyle name="40% - Accent6 2" xfId="41"/>
+    <cellStyle name="60% - Accent1 2" xfId="22"/>
+    <cellStyle name="60% - Accent2 2" xfId="26"/>
+    <cellStyle name="60% - Accent3 2" xfId="30"/>
+    <cellStyle name="60% - Accent4 2" xfId="34"/>
+    <cellStyle name="60% - Accent5 2" xfId="38"/>
+    <cellStyle name="60% - Accent6 2" xfId="42"/>
+    <cellStyle name="Accent1 2" xfId="19"/>
+    <cellStyle name="Accent2 2" xfId="23"/>
+    <cellStyle name="Accent3 2" xfId="27"/>
+    <cellStyle name="Accent4 2" xfId="31"/>
+    <cellStyle name="Accent5 2" xfId="35"/>
+    <cellStyle name="Accent6 2" xfId="39"/>
+    <cellStyle name="Bad 2" xfId="8"/>
+    <cellStyle name="Calculation 2" xfId="12"/>
+    <cellStyle name="Check Cell 2" xfId="14"/>
+    <cellStyle name="Explanatory Text 2" xfId="17"/>
+    <cellStyle name="Good 2" xfId="7"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input 2" xfId="10" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
-    <cellStyle name="Linked Cell 2" xfId="13" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
-    <cellStyle name="Neutral 2" xfId="9" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
+    <cellStyle name="Input 2" xfId="10"/>
+    <cellStyle name="Linked Cell 2" xfId="13"/>
+    <cellStyle name="Neutral 2" xfId="9"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="6" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
-    <cellStyle name="Note 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
-    <cellStyle name="Output 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
+    <cellStyle name="Normal 2" xfId="6"/>
+    <cellStyle name="Note 2" xfId="16"/>
+    <cellStyle name="Output 2" xfId="11"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
-    <cellStyle name="Warning Text 2" xfId="15" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
+    <cellStyle name="Total 2" xfId="18"/>
+    <cellStyle name="Warning Text 2" xfId="15"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1067,1105 +1082,1107 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3151121-9C59-4B6D-8B77-892B6EEA2D31}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B256"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="3">
         <v>174.0164</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>175.01975000000002</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>176.02310000000003</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>177.02645000000004</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>178.02980000000005</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>179.03315000000006</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>180.03650000000007</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>146.0215</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>147.02485000000001</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>148.02820000000003</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>149.03155000000004</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3">
         <v>150.03490000000005</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3">
         <v>151.03825000000006</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="3">
         <v>192.02699999999999</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="3">
         <v>193.03035</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="3">
         <v>194.03370000000001</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="3">
         <v>195.03705000000002</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="3">
         <v>196.04040000000003</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="3">
         <v>197.04375000000005</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="3">
         <v>198.04710000000006</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="3">
         <v>116.011</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="3">
         <v>117.01434999999999</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="3">
         <v>118.01769999999999</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="3">
         <v>119.02104999999999</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="3">
         <v>120.02439999999999</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="3">
         <v>147.0532</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="3">
         <v>148.05655000000002</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="3">
         <v>149.05990000000003</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="3">
         <v>150.06325000000004</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="3">
         <v>151.06660000000005</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="3">
         <v>152.06995000000006</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="3">
         <v>146.06909999999999</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="3">
         <v>147.07245</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="3">
         <v>148.07580000000002</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="3">
         <v>149.07915000000003</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="3">
         <v>150.08250000000004</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="3">
         <v>151.08585000000005</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="3">
         <v>192.02699999999999</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="3">
         <v>193.03035</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="3">
         <v>194.03370000000001</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="3">
         <v>195.03705000000002</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="3">
         <v>196.04040000000003</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="3">
         <v>197.04375000000005</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="3">
         <v>198.04710000000006</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="3">
         <v>134.0215</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="3">
         <v>135.02485000000001</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="3">
         <v>136.02820000000003</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="3">
         <v>137.03155000000004</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="3">
         <v>138.03490000000005</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="3">
         <v>132.0059</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="3">
         <v>133.00925000000001</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="3">
         <v>134.01260000000002</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="3">
         <v>135.01595000000003</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+      <c r="A54" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="3">
         <v>136.01930000000004</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+      <c r="A55" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="3">
         <v>867.13130000000001</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="3">
         <v>868.13464999999997</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+      <c r="A57" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="3">
         <v>869.13799999999992</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="3">
         <v>870.14134999999987</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+      <c r="A59" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="3">
         <v>871.14469999999983</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="3">
         <v>118.0266</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+      <c r="A61" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="3">
         <v>119.02995</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+      <c r="A62" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B62">
+      <c r="B62" s="3">
         <v>120.0333</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+      <c r="A63" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B63">
+      <c r="B63" s="3">
         <v>121.03664999999999</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B64">
+      <c r="B64" s="3">
         <v>122.03999999999999</v>
       </c>
     </row>
     <row r="65" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
+      <c r="A65" s="2"/>
     </row>
     <row r="66" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
+      <c r="A66" s="2"/>
     </row>
     <row r="67" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
+      <c r="A67" s="2"/>
     </row>
     <row r="68" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
+      <c r="A68" s="2"/>
     </row>
     <row r="69" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
+      <c r="A69" s="2"/>
     </row>
     <row r="70" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
+      <c r="A70" s="2"/>
     </row>
     <row r="71" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
+      <c r="A71" s="2"/>
     </row>
     <row r="72" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
+      <c r="A72" s="2"/>
     </row>
     <row r="73" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
+      <c r="A73" s="2"/>
     </row>
     <row r="74" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
+      <c r="A74" s="2"/>
     </row>
     <row r="75" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="1"/>
+      <c r="A75" s="2"/>
     </row>
     <row r="76" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="1"/>
+      <c r="A76" s="2"/>
     </row>
     <row r="77" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
+      <c r="A77" s="2"/>
     </row>
     <row r="78" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A78" s="1"/>
+      <c r="A78" s="2"/>
     </row>
     <row r="79" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A79" s="1"/>
+      <c r="A79" s="2"/>
     </row>
     <row r="80" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A80" s="1"/>
+      <c r="A80" s="2"/>
     </row>
     <row r="81" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A81" s="1"/>
+      <c r="A81" s="2"/>
     </row>
     <row r="82" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A82" s="1"/>
+      <c r="A82" s="2"/>
     </row>
     <row r="83" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A83" s="1"/>
+      <c r="A83" s="2"/>
     </row>
     <row r="84" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A84" s="1"/>
+      <c r="A84" s="2"/>
     </row>
     <row r="85" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
+      <c r="A85" s="2"/>
     </row>
     <row r="86" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A86" s="1"/>
+      <c r="A86" s="2"/>
     </row>
     <row r="87" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A87" s="1"/>
+      <c r="A87" s="2"/>
     </row>
     <row r="88" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A88" s="1"/>
+      <c r="A88" s="2"/>
     </row>
     <row r="89" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A89" s="1"/>
+      <c r="A89" s="2"/>
     </row>
     <row r="90" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A90" s="1"/>
+      <c r="A90" s="2"/>
     </row>
     <row r="91" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A91" s="1"/>
+      <c r="A91" s="2"/>
     </row>
     <row r="92" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A92" s="1"/>
+      <c r="A92" s="2"/>
     </row>
     <row r="93" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A93" s="1"/>
+      <c r="A93" s="2"/>
     </row>
     <row r="94" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A94" s="1"/>
+      <c r="A94" s="2"/>
     </row>
     <row r="95" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A95" s="1"/>
+      <c r="A95" s="2"/>
     </row>
     <row r="96" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A96" s="1"/>
+      <c r="A96" s="2"/>
     </row>
     <row r="97" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A97" s="1"/>
+      <c r="A97" s="2"/>
     </row>
     <row r="98" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A98" s="1"/>
+      <c r="A98" s="2"/>
     </row>
     <row r="99" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A99" s="1"/>
+      <c r="A99" s="2"/>
     </row>
     <row r="100" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A100" s="1"/>
+      <c r="A100" s="2"/>
     </row>
     <row r="101" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A101" s="1"/>
+      <c r="A101" s="2"/>
     </row>
     <row r="102" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A102" s="1"/>
+      <c r="A102" s="2"/>
     </row>
     <row r="103" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A103" s="1"/>
+      <c r="A103" s="2"/>
     </row>
     <row r="104" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A104" s="1"/>
+      <c r="A104" s="2"/>
     </row>
     <row r="105" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A105" s="1"/>
+      <c r="A105" s="2"/>
     </row>
     <row r="106" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A106" s="1"/>
+      <c r="A106" s="2"/>
     </row>
     <row r="107" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A107" s="1"/>
+      <c r="A107" s="2"/>
     </row>
     <row r="108" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A108" s="1"/>
+      <c r="A108" s="2"/>
     </row>
     <row r="109" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A109" s="1"/>
+      <c r="A109" s="2"/>
     </row>
     <row r="110" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A110" s="1"/>
+      <c r="A110" s="2"/>
     </row>
     <row r="111" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A111" s="1"/>
+      <c r="A111" s="2"/>
     </row>
     <row r="112" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A112" s="1"/>
+      <c r="A112" s="2"/>
     </row>
     <row r="113" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A113" s="1"/>
+      <c r="A113" s="2"/>
     </row>
     <row r="114" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A114" s="1"/>
+      <c r="A114" s="2"/>
     </row>
     <row r="115" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A115" s="1"/>
+      <c r="A115" s="2"/>
     </row>
     <row r="116" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A116" s="1"/>
+      <c r="A116" s="2"/>
     </row>
     <row r="117" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A117" s="1"/>
+      <c r="A117" s="2"/>
     </row>
     <row r="118" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A118" s="1"/>
+      <c r="A118" s="2"/>
     </row>
     <row r="119" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A119" s="1"/>
+      <c r="A119" s="2"/>
     </row>
     <row r="120" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A120" s="1"/>
+      <c r="A120" s="2"/>
     </row>
     <row r="121" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A121" s="1"/>
+      <c r="A121" s="2"/>
     </row>
     <row r="122" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A122" s="1"/>
+      <c r="A122" s="2"/>
     </row>
     <row r="123" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A123" s="1"/>
+      <c r="A123" s="2"/>
     </row>
     <row r="124" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A124" s="1"/>
+      <c r="A124" s="2"/>
     </row>
     <row r="125" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A125" s="1"/>
+      <c r="A125" s="2"/>
     </row>
     <row r="126" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A126" s="1"/>
+      <c r="A126" s="2"/>
     </row>
     <row r="127" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A127" s="1"/>
+      <c r="A127" s="2"/>
     </row>
     <row r="128" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A128" s="1"/>
+      <c r="A128" s="2"/>
     </row>
     <row r="129" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A129" s="1"/>
+      <c r="A129" s="2"/>
     </row>
     <row r="130" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A130" s="1"/>
+      <c r="A130" s="2"/>
     </row>
     <row r="131" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A131" s="1"/>
+      <c r="A131" s="2"/>
     </row>
     <row r="132" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A132" s="1"/>
+      <c r="A132" s="2"/>
     </row>
     <row r="133" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A133" s="1"/>
+      <c r="A133" s="2"/>
     </row>
     <row r="134" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A134" s="1"/>
+      <c r="A134" s="2"/>
     </row>
     <row r="135" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A135" s="1"/>
+      <c r="A135" s="2"/>
     </row>
     <row r="136" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A136" s="1"/>
+      <c r="A136" s="2"/>
     </row>
     <row r="137" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A137" s="1"/>
+      <c r="A137" s="2"/>
     </row>
     <row r="138" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A138" s="1"/>
+      <c r="A138" s="2"/>
     </row>
     <row r="139" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A139" s="1"/>
+      <c r="A139" s="2"/>
     </row>
     <row r="140" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A140" s="1"/>
+      <c r="A140" s="2"/>
     </row>
     <row r="141" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A141" s="1"/>
+      <c r="A141" s="2"/>
     </row>
     <row r="142" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A142" s="1"/>
+      <c r="A142" s="2"/>
     </row>
     <row r="143" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A143" s="1"/>
+      <c r="A143" s="2"/>
     </row>
     <row r="144" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A144" s="1"/>
+      <c r="A144" s="2"/>
     </row>
     <row r="145" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A145" s="1"/>
+      <c r="A145" s="2"/>
     </row>
     <row r="146" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A146" s="1"/>
+      <c r="A146" s="2"/>
     </row>
     <row r="147" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A147" s="1"/>
+      <c r="A147" s="2"/>
     </row>
     <row r="148" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A148" s="1"/>
+      <c r="A148" s="2"/>
     </row>
     <row r="149" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A149" s="1"/>
+      <c r="A149" s="2"/>
     </row>
     <row r="150" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A150" s="1"/>
+      <c r="A150" s="2"/>
     </row>
     <row r="151" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A151" s="1"/>
+      <c r="A151" s="2"/>
     </row>
     <row r="152" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A152" s="1"/>
+      <c r="A152" s="2"/>
     </row>
     <row r="153" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A153" s="1"/>
+      <c r="A153" s="2"/>
     </row>
     <row r="154" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A154" s="1"/>
+      <c r="A154" s="2"/>
     </row>
     <row r="155" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A155" s="1"/>
+      <c r="A155" s="2"/>
     </row>
     <row r="156" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A156" s="1"/>
+      <c r="A156" s="2"/>
     </row>
     <row r="157" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A157" s="1"/>
+      <c r="A157" s="2"/>
     </row>
     <row r="158" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A158" s="1"/>
+      <c r="A158" s="2"/>
     </row>
     <row r="159" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A159" s="1"/>
+      <c r="A159" s="2"/>
     </row>
     <row r="160" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A160" s="1"/>
+      <c r="A160" s="2"/>
     </row>
     <row r="161" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A161" s="1"/>
+      <c r="A161" s="2"/>
     </row>
     <row r="162" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A162" s="1"/>
+      <c r="A162" s="2"/>
     </row>
     <row r="163" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A163" s="1"/>
+      <c r="A163" s="2"/>
     </row>
     <row r="164" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A164" s="1"/>
+      <c r="A164" s="2"/>
     </row>
     <row r="165" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A165" s="1"/>
+      <c r="A165" s="2"/>
     </row>
     <row r="166" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A166" s="1"/>
+      <c r="A166" s="2"/>
     </row>
     <row r="167" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A167" s="1"/>
+      <c r="A167" s="2"/>
     </row>
     <row r="168" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A168" s="1"/>
+      <c r="A168" s="2"/>
     </row>
     <row r="169" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A169" s="1"/>
+      <c r="A169" s="2"/>
     </row>
     <row r="170" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A170" s="1"/>
+      <c r="A170" s="2"/>
     </row>
     <row r="171" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A171" s="1"/>
+      <c r="A171" s="2"/>
     </row>
     <row r="172" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A172" s="1"/>
+      <c r="A172" s="2"/>
     </row>
     <row r="173" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A173" s="1"/>
+      <c r="A173" s="2"/>
     </row>
     <row r="174" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A174" s="1"/>
+      <c r="A174" s="2"/>
     </row>
     <row r="175" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A175" s="1"/>
+      <c r="A175" s="2"/>
     </row>
     <row r="176" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A176" s="1"/>
+      <c r="A176" s="2"/>
     </row>
     <row r="177" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A177" s="1"/>
+      <c r="A177" s="2"/>
     </row>
     <row r="178" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A178" s="1"/>
+      <c r="A178" s="2"/>
     </row>
     <row r="179" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A179" s="1"/>
+      <c r="A179" s="2"/>
     </row>
     <row r="180" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A180" s="1"/>
+      <c r="A180" s="2"/>
     </row>
     <row r="181" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A181" s="1"/>
+      <c r="A181" s="2"/>
     </row>
     <row r="182" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A182" s="1"/>
+      <c r="A182" s="2"/>
     </row>
     <row r="183" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A183" s="1"/>
+      <c r="A183" s="2"/>
     </row>
     <row r="184" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A184" s="1"/>
+      <c r="A184" s="2"/>
     </row>
     <row r="185" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A185" s="1"/>
+      <c r="A185" s="2"/>
     </row>
     <row r="186" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A186" s="1"/>
+      <c r="A186" s="2"/>
     </row>
     <row r="187" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A187" s="1"/>
+      <c r="A187" s="2"/>
     </row>
     <row r="188" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A188" s="1"/>
+      <c r="A188" s="2"/>
     </row>
     <row r="189" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A189" s="1"/>
+      <c r="A189" s="2"/>
     </row>
     <row r="190" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A190" s="1"/>
+      <c r="A190" s="2"/>
     </row>
     <row r="191" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A191" s="1"/>
+      <c r="A191" s="2"/>
     </row>
     <row r="192" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A192" s="1"/>
+      <c r="A192" s="2"/>
     </row>
     <row r="193" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A193" s="1"/>
+      <c r="A193" s="2"/>
     </row>
     <row r="194" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A194" s="1"/>
+      <c r="A194" s="2"/>
     </row>
     <row r="195" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A195" s="1"/>
+      <c r="A195" s="2"/>
     </row>
     <row r="196" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A196" s="1"/>
+      <c r="A196" s="2"/>
     </row>
     <row r="197" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A197" s="1"/>
+      <c r="A197" s="2"/>
     </row>
     <row r="198" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A198" s="1"/>
+      <c r="A198" s="2"/>
     </row>
     <row r="199" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A199" s="1"/>
+      <c r="A199" s="2"/>
     </row>
     <row r="200" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A200" s="1"/>
+      <c r="A200" s="2"/>
     </row>
     <row r="201" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A201" s="1"/>
+      <c r="A201" s="2"/>
     </row>
     <row r="202" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A202" s="1"/>
+      <c r="A202" s="2"/>
     </row>
     <row r="203" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A203" s="1"/>
+      <c r="A203" s="2"/>
     </row>
     <row r="204" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A204" s="1"/>
+      <c r="A204" s="2"/>
     </row>
     <row r="205" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A205" s="1"/>
+      <c r="A205" s="2"/>
     </row>
     <row r="206" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A206" s="1"/>
+      <c r="A206" s="2"/>
     </row>
     <row r="207" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A207" s="1"/>
+      <c r="A207" s="2"/>
     </row>
     <row r="208" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A208" s="1"/>
+      <c r="A208" s="2"/>
     </row>
     <row r="209" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A209" s="1"/>
+      <c r="A209" s="2"/>
     </row>
     <row r="210" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A210" s="1"/>
+      <c r="A210" s="2"/>
     </row>
     <row r="211" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A211" s="1"/>
+      <c r="A211" s="2"/>
     </row>
     <row r="212" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A212" s="1"/>
+      <c r="A212" s="2"/>
     </row>
     <row r="213" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A213" s="1"/>
+      <c r="A213" s="2"/>
     </row>
     <row r="214" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A214" s="1"/>
+      <c r="A214" s="2"/>
     </row>
     <row r="215" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A215" s="1"/>
+      <c r="A215" s="2"/>
     </row>
     <row r="216" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A216" s="1"/>
+      <c r="A216" s="2"/>
     </row>
     <row r="217" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A217" s="1"/>
+      <c r="A217" s="2"/>
     </row>
     <row r="218" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A218" s="1"/>
+      <c r="A218" s="2"/>
     </row>
     <row r="219" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A219" s="1"/>
+      <c r="A219" s="2"/>
     </row>
     <row r="220" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A220" s="1"/>
+      <c r="A220" s="2"/>
     </row>
     <row r="221" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A221" s="1"/>
+      <c r="A221" s="2"/>
     </row>
     <row r="222" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A222" s="1"/>
+      <c r="A222" s="2"/>
     </row>
     <row r="223" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A223" s="1"/>
+      <c r="A223" s="2"/>
     </row>
     <row r="224" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A224" s="1"/>
+      <c r="A224" s="2"/>
     </row>
     <row r="225" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A225" s="1"/>
+      <c r="A225" s="2"/>
     </row>
     <row r="226" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A226" s="1"/>
+      <c r="A226" s="2"/>
     </row>
     <row r="227" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A227" s="1"/>
+      <c r="A227" s="2"/>
     </row>
     <row r="228" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A228" s="1"/>
+      <c r="A228" s="2"/>
     </row>
     <row r="229" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A229" s="1"/>
+      <c r="A229" s="2"/>
     </row>
     <row r="230" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A230" s="1"/>
+      <c r="A230" s="2"/>
     </row>
     <row r="231" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A231" s="1"/>
+      <c r="A231" s="2"/>
     </row>
     <row r="232" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A232" s="1"/>
+      <c r="A232" s="2"/>
     </row>
     <row r="233" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A233" s="1"/>
+      <c r="A233" s="2"/>
     </row>
     <row r="234" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A234" s="1"/>
+      <c r="A234" s="2"/>
     </row>
     <row r="235" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A235" s="1"/>
+      <c r="A235" s="2"/>
     </row>
     <row r="236" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A236" s="1"/>
+      <c r="A236" s="2"/>
     </row>
     <row r="237" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A237" s="1"/>
+      <c r="A237" s="2"/>
     </row>
     <row r="238" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A238" s="1"/>
+      <c r="A238" s="2"/>
     </row>
     <row r="239" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A239" s="1"/>
+      <c r="A239" s="2"/>
     </row>
     <row r="240" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A240" s="1"/>
+      <c r="A240" s="2"/>
     </row>
     <row r="241" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A241" s="1"/>
+      <c r="A241" s="2"/>
     </row>
     <row r="242" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A242" s="1"/>
+      <c r="A242" s="2"/>
     </row>
     <row r="243" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A243" s="1"/>
+      <c r="A243" s="2"/>
     </row>
     <row r="244" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A244" s="1"/>
+      <c r="A244" s="2"/>
     </row>
     <row r="245" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A245" s="1"/>
+      <c r="A245" s="2"/>
     </row>
     <row r="246" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A246" s="1"/>
+      <c r="A246" s="2"/>
     </row>
     <row r="247" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A247" s="1"/>
+      <c r="A247" s="2"/>
     </row>
     <row r="248" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A248" s="1"/>
+      <c r="A248" s="2"/>
     </row>
     <row r="249" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A249" s="1"/>
+      <c r="A249" s="2"/>
     </row>
     <row r="250" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A250" s="1"/>
+      <c r="A250" s="2"/>
     </row>
     <row r="251" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A251" s="1"/>
+      <c r="A251" s="2"/>
     </row>
     <row r="252" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A252" s="1"/>
+      <c r="A252" s="2"/>
     </row>
     <row r="253" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A253" s="1"/>
+      <c r="A253" s="2"/>
     </row>
     <row r="254" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A254" s="1"/>
+      <c r="A254" s="2"/>
     </row>
     <row r="255" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A255" s="1"/>
+      <c r="A255" s="2"/>
     </row>
     <row r="256" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A256" s="1"/>
+      <c r="A256" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>